<commit_message>
made changes to spreadsheet
</commit_message>
<xml_diff>
--- a/formal_concept.xlsx
+++ b/formal_concept.xlsx
@@ -16,14 +16,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
   <si>
     <t>bird</t>
   </si>
   <si>
-    <t>aithyia</t>
-  </si>
-  <si>
     <t>web-footed</t>
   </si>
   <si>
@@ -48,10 +45,43 @@
     <t>dive into the sea</t>
   </si>
   <si>
-    <t>apotheosis/heroization</t>
-  </si>
-  <si>
     <t>yes</t>
+  </si>
+  <si>
+    <t>aithyia (gull)</t>
+  </si>
+  <si>
+    <t>memnon (ruff)</t>
+  </si>
+  <si>
+    <t>unknown</t>
+  </si>
+  <si>
+    <t>ortyx (quail)</t>
+  </si>
+  <si>
+    <t>erodioi(herons)</t>
+  </si>
+  <si>
+    <t>erodioi(shearwaters)</t>
+  </si>
+  <si>
+    <t>myth</t>
+  </si>
+  <si>
+    <t>Ino</t>
+  </si>
+  <si>
+    <t>Companions of Memnon</t>
+  </si>
+  <si>
+    <t>Asteria</t>
+  </si>
+  <si>
+    <t>Companions of Diomedes</t>
+  </si>
+  <si>
+    <t>Companions of Diomedes (after recant in 1918)</t>
   </si>
 </sst>
 </file>
@@ -383,14 +413,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
+    <col min="1" max="1" width="18.7109375" customWidth="1"/>
     <col min="2" max="2" width="12.140625" customWidth="1"/>
     <col min="5" max="5" width="12.7109375" customWidth="1"/>
     <col min="9" max="9" width="18" customWidth="1"/>
@@ -402,48 +433,107 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="I1" t="s">
-        <v>9</v>
-      </c>
       <c r="J1" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" t="s">
         <v>11</v>
       </c>
-      <c r="G2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2" t="s">
-        <v>11</v>
-      </c>
-      <c r="J2" t="s">
-        <v>11</v>
+      <c r="H3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" t="s">
+        <v>9</v>
+      </c>
+      <c r="J5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6" t="s">
+        <v>9</v>
+      </c>
+      <c r="J6" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>